<commit_message>
A little formatting of excel file.
</commit_message>
<xml_diff>
--- a/PBJ_EU/pbj_eu.xlsx
+++ b/PBJ_EU/pbj_eu.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Shannon\Dropbox\moog\PBJ\PBJ_EU\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shann\Dropbox\moog\PBJ\PBJ_EU\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{083D1D8E-27D4-4C1D-8A93-F295078EAFA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A57EC47-841E-4605-9550-A430F9500B95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1075,6 +1075,8 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
+    <col min="1" max="1" width="33.5703125" customWidth="1"/>
+    <col min="2" max="2" width="11.85546875" customWidth="1"/>
     <col min="3" max="3" width="48.7109375" customWidth="1"/>
     <col min="4" max="5" width="29.28515625" customWidth="1"/>
   </cols>

</xml_diff>